<commit_message>
Adding additional cpra station locations as requested.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Gate_Closure_Trigger.xlsx
+++ b/output/cpra_postproc/Gate_Closure_Trigger.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>17StCanal</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Hero Canal Stop-Log Gate</t>
+  </si>
+  <si>
+    <t>LakefrontAirport</t>
+  </si>
+  <si>
+    <t>Mandeville</t>
+  </si>
+  <si>
+    <t>Rigolets</t>
+  </si>
+  <si>
+    <t>Lafitte</t>
+  </si>
+  <si>
+    <t>Lakefront Airport</t>
   </si>
 </sst>
 </file>
@@ -418,12 +433,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -559,6 +575,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adjusting CPRA gate closure triggers based on feedback from CPRA.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Gate_Closure_Trigger.xlsx
+++ b/output/cpra_postproc/Gate_Closure_Trigger.xlsx
@@ -435,7 +435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -451,7 +453,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -539,7 +541,7 @@
         <v>19</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -561,7 +563,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Adding timeout option of 20 seconds when attempting to download xml files from rivergages.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Gate_Closure_Trigger.xlsx
+++ b/output/cpra_postproc/Gate_Closure_Trigger.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\asgs\output\cpra_postproc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CPRA_Manual\Adv12\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,7 +475,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,7 +519,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -552,7 +552,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixing typo in Boomtown Casio and updating Gate Closure Excel file.
</commit_message>
<xml_diff>
--- a/output/cpra_postproc/Gate_Closure_Trigger.xlsx
+++ b/output/cpra_postproc/Gate_Closure_Trigger.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CPRA_Manual\Adv12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbilsk3\Documents\PROJECTS\CPRA\asgs\output\cpra_postproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427BB8C5-7D50-4B6A-B1DF-5679D9B3E481}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="8400" yWindow="936" windowWidth="12438" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>17StCanal</t>
   </si>
@@ -111,12 +112,48 @@
   </si>
   <si>
     <t>Lakefront Airport</t>
+  </si>
+  <si>
+    <t>HarveyCanalNorth</t>
+  </si>
+  <si>
+    <t>HarveyCanalBoom</t>
+  </si>
+  <si>
+    <t>BayouBienv</t>
+  </si>
+  <si>
+    <t>BaraPass</t>
+  </si>
+  <si>
+    <t>FreshCanal</t>
+  </si>
+  <si>
+    <t>CalcRiv</t>
+  </si>
+  <si>
+    <t>Harvey Canal Sector Gates North / Prot Side nr Lapalco Blvd</t>
+  </si>
+  <si>
+    <t>Harvey Canal at Boomtown Casion</t>
+  </si>
+  <si>
+    <t>Bayou Bienvenue Floodgate</t>
+  </si>
+  <si>
+    <t>Barataria Pass at Grand Isle</t>
+  </si>
+  <si>
+    <t>Freshwater Canal at Freshwater Bayou Lock South</t>
+  </si>
+  <si>
+    <t>Calcasieu River at Cameron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -432,20 +469,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.9453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -467,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -478,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -489,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -500,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -511,7 +548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -522,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -533,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -544,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -555,7 +592,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -566,7 +603,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -577,7 +614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -588,7 +625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -599,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -610,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -618,6 +655,72 @@
         <v>27</v>
       </c>
       <c r="C16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>